<commit_message>
MEB values percentage change
</commit_message>
<xml_diff>
--- a/outputs/UG_Covid_jmmi_15may2020_safety reasons.xlsx
+++ b/outputs/UG_Covid_jmmi_15may2020_safety reasons.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t xml:space="preserve">Regions</t>
   </si>
@@ -51,27 +51,27 @@
     <t xml:space="preserve">Markets less crowded</t>
   </si>
   <si>
+    <t xml:space="preserve">Introduction of new rules and regulations</t>
+  </si>
+  <si>
     <t xml:space="preserve">No theft</t>
   </si>
   <si>
-    <t xml:space="preserve">Introduction of new rules and regulations</t>
-  </si>
-  <si>
     <t xml:space="preserve">Relaxation of rules and regulations</t>
   </si>
   <si>
+    <t xml:space="preserve">Installation of sanitary infrastructure</t>
+  </si>
+  <si>
     <t xml:space="preserve">n/a</t>
   </si>
   <si>
-    <t xml:space="preserve">Installation of sanitary infrastructure</t>
+    <t xml:space="preserve">Appropriate behaviour of security personnel</t>
   </si>
   <si>
     <t xml:space="preserve">Reduced threats of disease spread</t>
   </si>
   <si>
-    <t xml:space="preserve">Appropriate behaviour of security personnel</t>
-  </si>
-  <si>
     <t xml:space="preserve">No threats of covic infections</t>
   </si>
   <si>
@@ -90,31 +90,28 @@
     <t xml:space="preserve">Fear of theft </t>
   </si>
   <si>
+    <t xml:space="preserve">Fear of contracting COVID-19</t>
+  </si>
+  <si>
     <t xml:space="preserve">Non-compliance with official rules and regulations</t>
   </si>
   <si>
-    <t xml:space="preserve">Fear of contracting COVID-19</t>
+    <t xml:space="preserve">Discretionary behaviour of security personnel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Some people stopped working and may pose a big threat to our merchandise</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Corona-infected individuals in the area</t>
   </si>
   <si>
     <t xml:space="preserve">Health risks in relation to COVID-19</t>
   </si>
   <si>
-    <t xml:space="preserve">Discretionary behaviour of security personnel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fear of contracting COVID-20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Some people stopped working and may pose a big threat to our merchandise</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Corona-infected individuals in the area</t>
+    <t xml:space="preserve">Lack of customers</t>
   </si>
   <si>
     <t xml:space="preserve">Restrictive rules and regulations</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lack of customers</t>
   </si>
 </sst>
 </file>
@@ -474,7 +471,7 @@
         <v>7</v>
       </c>
       <c r="D2" t="n">
-        <v>0.326086956521739</v>
+        <v>0.326530612244898</v>
       </c>
       <c r="E2" t="n">
         <v>1</v>
@@ -491,7 +488,7 @@
         <v>8</v>
       </c>
       <c r="D3" t="n">
-        <v>0.173913043478261</v>
+        <v>0.204081632653061</v>
       </c>
       <c r="E3" t="n">
         <v>2</v>
@@ -508,7 +505,7 @@
         <v>9</v>
       </c>
       <c r="D4" t="n">
-        <v>0.152173913043478</v>
+        <v>0.142857142857143</v>
       </c>
       <c r="E4" t="n">
         <v>3</v>
@@ -525,7 +522,7 @@
         <v>10</v>
       </c>
       <c r="D5" t="n">
-        <v>0.108695652173913</v>
+        <v>0.102040816326531</v>
       </c>
       <c r="E5" t="n">
         <v>4</v>
@@ -542,7 +539,7 @@
         <v>11</v>
       </c>
       <c r="D6" t="n">
-        <v>0.0652173913043478</v>
+        <v>0.0612244897959184</v>
       </c>
       <c r="E6" t="n">
         <v>5</v>
@@ -559,7 +556,7 @@
         <v>12</v>
       </c>
       <c r="D7" t="n">
-        <v>0.0434782608695652</v>
+        <v>0.0408163265306122</v>
       </c>
       <c r="E7" t="n">
         <v>6</v>
@@ -576,7 +573,7 @@
         <v>13</v>
       </c>
       <c r="D8" t="n">
-        <v>0.0434782608695652</v>
+        <v>0.0408163265306122</v>
       </c>
       <c r="E8" t="n">
         <v>7</v>
@@ -593,7 +590,7 @@
         <v>14</v>
       </c>
       <c r="D9" t="n">
-        <v>0.0434782608695652</v>
+        <v>0.0408163265306122</v>
       </c>
       <c r="E9" t="n">
         <v>8</v>
@@ -610,7 +607,7 @@
         <v>15</v>
       </c>
       <c r="D10" t="n">
-        <v>0.0217391304347826</v>
+        <v>0.0204081632653061</v>
       </c>
       <c r="E10" t="n">
         <v>9</v>
@@ -627,7 +624,7 @@
         <v>16</v>
       </c>
       <c r="D11" t="n">
-        <v>0.0217391304347826</v>
+        <v>0.0204081632653061</v>
       </c>
       <c r="E11" t="n">
         <v>10</v>
@@ -743,7 +740,7 @@
         <v>6</v>
       </c>
       <c r="C18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D18" t="n">
         <v>0.111111111111111</v>
@@ -794,7 +791,7 @@
         <v>6</v>
       </c>
       <c r="C21" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D21" t="n">
         <v>0</v>
@@ -811,7 +808,7 @@
         <v>6</v>
       </c>
       <c r="C22" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D22" t="n">
         <v>0</v>
@@ -828,7 +825,7 @@
         <v>6</v>
       </c>
       <c r="C23" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D23" t="n">
         <v>0</v>
@@ -845,7 +842,7 @@
         <v>6</v>
       </c>
       <c r="C24" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D24" t="n">
         <v>0</v>
@@ -862,7 +859,7 @@
         <v>6</v>
       </c>
       <c r="C25" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D25" t="n">
         <v>0</v>
@@ -916,7 +913,7 @@
         <v>7</v>
       </c>
       <c r="D28" t="n">
-        <v>0.297297297297297</v>
+        <v>0.3</v>
       </c>
       <c r="E28" t="n">
         <v>1</v>
@@ -933,7 +930,7 @@
         <v>8</v>
       </c>
       <c r="D29" t="n">
-        <v>0.189189189189189</v>
+        <v>0.225</v>
       </c>
       <c r="E29" t="n">
         <v>2</v>
@@ -950,7 +947,7 @@
         <v>9</v>
       </c>
       <c r="D30" t="n">
-        <v>0.162162162162162</v>
+        <v>0.15</v>
       </c>
       <c r="E30" t="n">
         <v>3</v>
@@ -967,7 +964,7 @@
         <v>11</v>
       </c>
       <c r="D31" t="n">
-        <v>0.0810810810810811</v>
+        <v>0.075</v>
       </c>
       <c r="E31" t="n">
         <v>4</v>
@@ -984,7 +981,7 @@
         <v>10</v>
       </c>
       <c r="D32" t="n">
-        <v>0.0810810810810811</v>
+        <v>0.075</v>
       </c>
       <c r="E32" t="n">
         <v>5</v>
@@ -998,10 +995,10 @@
         <v>6</v>
       </c>
       <c r="C33" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D33" t="n">
-        <v>0.0540540540540541</v>
+        <v>0.05</v>
       </c>
       <c r="E33" t="n">
         <v>6</v>
@@ -1015,10 +1012,10 @@
         <v>6</v>
       </c>
       <c r="C34" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D34" t="n">
-        <v>0.0540540540540541</v>
+        <v>0.05</v>
       </c>
       <c r="E34" t="n">
         <v>7</v>
@@ -1032,10 +1029,10 @@
         <v>6</v>
       </c>
       <c r="C35" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D35" t="n">
-        <v>0.027027027027027</v>
+        <v>0.025</v>
       </c>
       <c r="E35" t="n">
         <v>8</v>
@@ -1052,7 +1049,7 @@
         <v>15</v>
       </c>
       <c r="D36" t="n">
-        <v>0.027027027027027</v>
+        <v>0.025</v>
       </c>
       <c r="E36" t="n">
         <v>9</v>
@@ -1066,10 +1063,10 @@
         <v>6</v>
       </c>
       <c r="C37" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D37" t="n">
-        <v>0.027027027027027</v>
+        <v>0.025</v>
       </c>
       <c r="E37" t="n">
         <v>10</v>
@@ -1083,7 +1080,7 @@
         <v>6</v>
       </c>
       <c r="C38" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D38" t="n">
         <v>0</v>
@@ -1100,7 +1097,7 @@
         <v>6</v>
       </c>
       <c r="C39" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D39" t="n">
         <v>0</v>
@@ -1168,7 +1165,7 @@
         <v>24</v>
       </c>
       <c r="D2" t="n">
-        <v>0.333333333333333</v>
+        <v>0.318181818181818</v>
       </c>
       <c r="E2" t="n">
         <v>1</v>
@@ -1185,7 +1182,7 @@
         <v>25</v>
       </c>
       <c r="D3" t="n">
-        <v>0.238095238095238</v>
+        <v>0.227272727272727</v>
       </c>
       <c r="E3" t="n">
         <v>2</v>
@@ -1202,7 +1199,7 @@
         <v>26</v>
       </c>
       <c r="D4" t="n">
-        <v>0.19047619047619</v>
+        <v>0.227272727272727</v>
       </c>
       <c r="E4" t="n">
         <v>3</v>
@@ -1219,7 +1216,7 @@
         <v>27</v>
       </c>
       <c r="D5" t="n">
-        <v>0.0476190476190476</v>
+        <v>0.0909090909090909</v>
       </c>
       <c r="E5" t="n">
         <v>4</v>
@@ -1236,7 +1233,7 @@
         <v>28</v>
       </c>
       <c r="D6" t="n">
-        <v>0.0476190476190476</v>
+        <v>0.0454545454545455</v>
       </c>
       <c r="E6" t="n">
         <v>5</v>
@@ -1253,7 +1250,7 @@
         <v>29</v>
       </c>
       <c r="D7" t="n">
-        <v>0.0476190476190476</v>
+        <v>0.0454545454545455</v>
       </c>
       <c r="E7" t="n">
         <v>6</v>
@@ -1270,7 +1267,7 @@
         <v>30</v>
       </c>
       <c r="D8" t="n">
-        <v>0.0476190476190476</v>
+        <v>0.0454545454545455</v>
       </c>
       <c r="E8" t="n">
         <v>7</v>
@@ -1287,7 +1284,7 @@
         <v>31</v>
       </c>
       <c r="D9" t="n">
-        <v>0.0476190476190476</v>
+        <v>0</v>
       </c>
       <c r="E9" t="n">
         <v>8</v>
@@ -1329,19 +1326,19 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="B12" t="s">
         <v>6</v>
       </c>
       <c r="C12" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="D12" t="n">
-        <v>0</v>
+        <v>0.363636363636364</v>
       </c>
       <c r="E12" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13">
@@ -1358,7 +1355,7 @@
         <v>0.363636363636364</v>
       </c>
       <c r="E13" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14">
@@ -1369,13 +1366,13 @@
         <v>6</v>
       </c>
       <c r="C14" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D14" t="n">
-        <v>0.272727272727273</v>
+        <v>0.0909090909090909</v>
       </c>
       <c r="E14" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15">
@@ -1386,13 +1383,13 @@
         <v>6</v>
       </c>
       <c r="C15" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D15" t="n">
         <v>0.0909090909090909</v>
       </c>
       <c r="E15" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="16">
@@ -1403,13 +1400,13 @@
         <v>6</v>
       </c>
       <c r="C16" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D16" t="n">
         <v>0.0909090909090909</v>
       </c>
       <c r="E16" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17">
@@ -1420,13 +1417,13 @@
         <v>6</v>
       </c>
       <c r="C17" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D17" t="n">
-        <v>0.0909090909090909</v>
+        <v>0</v>
       </c>
       <c r="E17" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="18">
@@ -1437,13 +1434,13 @@
         <v>6</v>
       </c>
       <c r="C18" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D18" t="n">
-        <v>0.0909090909090909</v>
+        <v>0</v>
       </c>
       <c r="E18" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="19">
@@ -1454,13 +1451,13 @@
         <v>6</v>
       </c>
       <c r="C19" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="D19" t="n">
         <v>0</v>
       </c>
       <c r="E19" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="20">
@@ -1471,13 +1468,13 @@
         <v>6</v>
       </c>
       <c r="C20" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="D20" t="n">
         <v>0</v>
       </c>
       <c r="E20" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="21">
@@ -1488,47 +1485,47 @@
         <v>6</v>
       </c>
       <c r="C21" t="s">
-        <v>32</v>
+        <v>7</v>
       </c>
       <c r="D21" t="n">
         <v>0</v>
       </c>
       <c r="E21" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B22" t="s">
         <v>6</v>
       </c>
       <c r="C22" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="D22" t="n">
-        <v>0</v>
+        <v>0.363636363636364</v>
       </c>
       <c r="E22" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B23" t="s">
         <v>6</v>
       </c>
       <c r="C23" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D23" t="n">
-        <v>0</v>
+        <v>0.272727272727273</v>
       </c>
       <c r="E23" t="n">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="24">
@@ -1539,13 +1536,13 @@
         <v>6</v>
       </c>
       <c r="C24" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D24" t="n">
-        <v>0.4</v>
+        <v>0.181818181818182</v>
       </c>
       <c r="E24" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="25">
@@ -1556,13 +1553,13 @@
         <v>6</v>
       </c>
       <c r="C25" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="D25" t="n">
-        <v>0.3</v>
+        <v>0.0909090909090909</v>
       </c>
       <c r="E25" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="26">
@@ -1573,13 +1570,13 @@
         <v>6</v>
       </c>
       <c r="C26" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D26" t="n">
-        <v>0.1</v>
+        <v>0.0909090909090909</v>
       </c>
       <c r="E26" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="27">
@@ -1590,13 +1587,13 @@
         <v>6</v>
       </c>
       <c r="C27" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="D27" t="n">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="E27" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="28">
@@ -1607,13 +1604,13 @@
         <v>6</v>
       </c>
       <c r="C28" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="D28" t="n">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="E28" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="29">
@@ -1624,13 +1621,13 @@
         <v>6</v>
       </c>
       <c r="C29" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D29" t="n">
         <v>0</v>
       </c>
       <c r="E29" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="30">
@@ -1641,13 +1638,13 @@
         <v>6</v>
       </c>
       <c r="C30" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D30" t="n">
         <v>0</v>
       </c>
       <c r="E30" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="31">
@@ -1658,64 +1655,13 @@
         <v>6</v>
       </c>
       <c r="C31" t="s">
-        <v>7</v>
+        <v>31</v>
       </c>
       <c r="D31" t="n">
         <v>0</v>
       </c>
       <c r="E31" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="s">
-        <v>21</v>
-      </c>
-      <c r="B32" t="s">
-        <v>6</v>
-      </c>
-      <c r="C32" t="s">
-        <v>29</v>
-      </c>
-      <c r="D32" t="n">
-        <v>0</v>
-      </c>
-      <c r="E32" t="n">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="s">
-        <v>21</v>
-      </c>
-      <c r="B33" t="s">
-        <v>6</v>
-      </c>
-      <c r="C33" t="s">
-        <v>30</v>
-      </c>
-      <c r="D33" t="n">
-        <v>0</v>
-      </c>
-      <c r="E33" t="n">
         <v>10</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="s">
-        <v>21</v>
-      </c>
-      <c r="B34" t="s">
-        <v>6</v>
-      </c>
-      <c r="C34" t="s">
-        <v>32</v>
-      </c>
-      <c r="D34" t="n">
-        <v>0</v>
-      </c>
-      <c r="E34" t="n">
-        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>